<commit_message>
Subir carpeta bases datos
</commit_message>
<xml_diff>
--- a/Base de Datos/Diccionario de Datos/Formato Diccionario de Datos - copia.xlsx
+++ b/Base de Datos/Diccionario de Datos/Formato Diccionario de Datos - copia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jupin\Documents\Laboral SENA\Formacion\Contenidos Formacion\Bases de Datos\Trimestre II - MYSQL\Diccionario de Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis Miguel\Documents\Repositorio SENA\ADSO2873707_PROGRAMACION\Base de Datos\Diccionario de Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF05A20-0790-40F1-AECB-CFF78DD849B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2940EB15-C738-49C5-9005-0397FEA86934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diccionario de Datos" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="24">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -54,127 +54,49 @@
     <t xml:space="preserve">DICCIONARIO DE DATOS </t>
   </si>
   <si>
-    <t>direccion</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Base datos: bd_pedidos</t>
-  </si>
-  <si>
-    <t>TABLA : cliente</t>
-  </si>
-  <si>
-    <t>codCliente</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Saldo</t>
-  </si>
-  <si>
-    <t>LimiteCredito</t>
-  </si>
-  <si>
-    <t>Descuento</t>
-  </si>
-  <si>
-    <t>MEDIUMINT</t>
-  </si>
-  <si>
-    <t>Llave primaria que identifica un cliente</t>
-  </si>
-  <si>
-    <t>VARCHAR</t>
-  </si>
-  <si>
     <t>[0-9]</t>
   </si>
   <si>
-    <t>Nombre del usuario cliente</t>
-  </si>
-  <si>
-    <t>[a-z][A-Z]</t>
-  </si>
-  <si>
-    <t>FLOAT</t>
-  </si>
-  <si>
-    <t>Identifica lo que el cliente debe</t>
-  </si>
-  <si>
-    <t>Reprenta el valor máximo que un cliente puede prestar</t>
-  </si>
-  <si>
-    <t>Representa el valor de descuento en las compras para el cliente</t>
-  </si>
-  <si>
     <t>TABLA : direccion</t>
   </si>
   <si>
-    <t>NorDireccion</t>
-  </si>
-  <si>
-    <t>comuna</t>
-  </si>
-  <si>
-    <t>calle</t>
-  </si>
-  <si>
-    <t>ciudad</t>
-  </si>
-  <si>
-    <t>Llave primera que identifica una dirección de envío</t>
-  </si>
-  <si>
-    <t>[a-z][A-Z][0-9][ - | # | . ]</t>
-  </si>
-  <si>
-    <t>Comuna del municipio del envío</t>
-  </si>
-  <si>
-    <t>[a-z][A-Z][0-9]</t>
-  </si>
-  <si>
     <t>TABLA : cliente_direccion</t>
   </si>
   <si>
     <t>TABLA : c</t>
   </si>
   <si>
-    <t>FkCodCliente</t>
-  </si>
-  <si>
-    <t>FkNrDireccion</t>
-  </si>
-  <si>
-    <t>Llave foránea de la tabla cliente</t>
-  </si>
-  <si>
-    <t>Llave foránea de la tabla Direccion</t>
-  </si>
-  <si>
     <t>TABLA : pedido</t>
   </si>
   <si>
-    <t>codPedido</t>
-  </si>
-  <si>
-    <t>BIGINT</t>
-  </si>
-  <si>
-    <t>FechaPedido</t>
-  </si>
-  <si>
-    <t>FechaEntrega</t>
-  </si>
-  <si>
-    <t>DATETIME</t>
-  </si>
-  <si>
-    <t>"aaaa-mm-dd H:i:s"</t>
+    <t>Base datos: articulos_db</t>
+  </si>
+  <si>
+    <t>TABLA : usuario</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>idUsuario</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>telefono</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>genero</t>
+  </si>
+  <si>
+    <t>INT</t>
   </si>
 </sst>
 </file>
@@ -449,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -477,21 +399,45 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -499,36 +445,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -839,24 +755,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="1" customWidth="1"/>
-    <col min="4" max="7" width="11.42578125" style="1"/>
-    <col min="8" max="8" width="55.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="45.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="1" customWidth="1"/>
+    <col min="4" max="7" width="11.44140625" style="1"/>
+    <col min="8" max="8" width="55.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="5"/>
@@ -868,61 +784,61 @@
       <c r="I1" s="5"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="B2" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="18"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="26"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
-      <c r="B5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15"/>
+      <c r="B5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="21"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="6" t="s">
         <v>0</v>
@@ -950,575 +866,445 @@
       </c>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
-      <c r="B7" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="11"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="22">
-        <v>10</v>
-      </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="24" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="22">
-        <v>80</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="4"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="23">
-        <v>10</v>
-      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>21</v>
-      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="12"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
-      <c r="B10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="23">
-        <v>10</v>
-      </c>
+      <c r="B10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" s="20" t="s">
+      <c r="H10" s="9"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="23">
-        <v>10</v>
-      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="20" t="s">
-        <v>21</v>
-      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="12"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="B12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="12"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
-      <c r="B13" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="15"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C15" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G15" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="2">
-        <v>80</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I15" s="27" t="s">
-        <v>34</v>
-      </c>
       <c r="J15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
-      <c r="B16" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="2">
-        <v>30</v>
-      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="F16" s="11"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>36</v>
-      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="17"/>
       <c r="J16" s="4"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
-      <c r="B17" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="2">
-        <v>30</v>
-      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="9"/>
-      <c r="I17" s="27"/>
+      <c r="I17" s="12"/>
       <c r="J17" s="4"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
-      <c r="B18" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="2">
-        <v>50</v>
-      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="9"/>
-      <c r="I18" s="27"/>
+      <c r="I18" s="17"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="17"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
-      <c r="B20" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="15"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
       <c r="J20" s="4"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D22" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E22" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F22" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H22" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I22" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="22">
-        <v>10</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I22" s="20" t="s">
-        <v>21</v>
-      </c>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
-      <c r="B23" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="2">
-        <v>80</v>
-      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I23" s="20" t="s">
-        <v>21</v>
-      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="12"/>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="12"/>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
-      <c r="B25" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="15"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G27" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H27" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I26" s="8" t="s">
+      <c r="I27" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J26" s="4"/>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="2">
-        <v>11</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="10"/>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
-      <c r="B28" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="2">
-        <v>80</v>
-      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="F28" s="11"/>
       <c r="G28" s="2"/>
       <c r="H28" s="9"/>
       <c r="I28" s="10"/>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
-      <c r="B29" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="9"/>
-      <c r="I29" s="10" t="s">
-        <v>49</v>
-      </c>
+      <c r="I29" s="10"/>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
-      <c r="B30" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="9"/>
-      <c r="I30" s="10" t="s">
-        <v>49</v>
-      </c>
+      <c r="I30" s="10"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
-      <c r="B31" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="22">
-        <v>10</v>
-      </c>
+      <c r="B31" s="16"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="19" t="s">
-        <v>10</v>
-      </c>
+      <c r="G31" s="2"/>
       <c r="H31" s="9"/>
       <c r="I31" s="10"/>
       <c r="J31" s="4"/>
     </row>
-    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="10"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
-      <c r="B33" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="15"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
       <c r="J33" s="4"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4"/>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="4"/>
+      <c r="B35" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C35" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D35" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E35" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F35" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="G35" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H34" s="7" t="s">
+      <c r="H35" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I34" s="8" t="s">
+      <c r="I35" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J34" s="4"/>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="10"/>
       <c r="J35" s="4"/>
     </row>
-    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="C36" s="2"/>
@@ -1530,7 +1316,7 @@
       <c r="I36" s="10"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="2"/>
@@ -1542,7 +1328,7 @@
       <c r="I37" s="10"/>
       <c r="J37" s="4"/>
     </row>
-    <row r="38" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="2"/>
@@ -1554,73 +1340,73 @@
       <c r="I38" s="10"/>
       <c r="J38" s="4"/>
     </row>
-    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="10"/>
       <c r="J39" s="4"/>
     </row>
-    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4"/>
-      <c r="B40" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="15"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
       <c r="J40" s="4"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4"/>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="4"/>
+      <c r="B42" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C42" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D42" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E42" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="F42" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G41" s="7" t="s">
+      <c r="G42" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H41" s="7" t="s">
+      <c r="H42" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I41" s="8" t="s">
+      <c r="I42" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J41" s="4"/>
-    </row>
-    <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="10"/>
       <c r="J42" s="4"/>
     </row>
-    <row r="43" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="C43" s="2"/>
@@ -1632,7 +1418,7 @@
       <c r="I43" s="10"/>
       <c r="J43" s="4"/>
     </row>
-    <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="4"/>
       <c r="B44" s="3"/>
       <c r="C44" s="2"/>
@@ -1644,7 +1430,7 @@
       <c r="I44" s="10"/>
       <c r="J44" s="4"/>
     </row>
-    <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="C45" s="2"/>
@@ -1656,19 +1442,19 @@
       <c r="I45" s="10"/>
       <c r="J45" s="4"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="10"/>
       <c r="J46" s="4"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1680,16 +1466,28 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
     </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="B25:I25"/>
-    <mergeCell ref="B33:I33"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="B34:I34"/>
     <mergeCell ref="B2:I3"/>
-    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:I14"/>
     <mergeCell ref="B4:I4"/>
     <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B40:I40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1697,6 +1495,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002036A9F4E641174895EF4CF963CE38EB" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="19e261f8c698451b5a55409c2375a187">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="31d5eec3c12ee2e8127422d567928fa7">
     <xsd:element name="properties">
@@ -1810,19 +1617,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E299484-3887-4E12-982B-31DC2EB2F666}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25543F57-B1BE-42AD-9380-EC75BA3D3C59}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25543F57-B1BE-42AD-9380-EC75BA3D3C59}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E299484-3887-4E12-982B-31DC2EB2F666}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>